<commit_message>
se agregaron predicciones para el mejor modelo de consumo de combustibles regular y super
</commit_message>
<xml_diff>
--- a/Estadisticas.xlsx
+++ b/Estadisticas.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pabloherrera/Documents/Universidad/Data Science/Laboratorio 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanluis/Documents/educacion/U/semestres/semestre_10/Datasci/Laboratorio-Series-Temporales/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8331BC16-EB6D-A041-8735-B41879DEFE64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF221DED-DA54-3A48-B98A-E05740C7FB48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="680" windowWidth="14180" windowHeight="17180" xr2:uid="{E6251B29-31E4-684F-AE2D-389F1F022EA4}"/>
+    <workbookView xWindow="1400" yWindow="760" windowWidth="14180" windowHeight="17180" activeTab="2" xr2:uid="{E6251B29-31E4-684F-AE2D-389F1F022EA4}"/>
   </bookViews>
   <sheets>
     <sheet name="IMPORTACION" sheetId="1" r:id="rId1"/>
     <sheet name="CONSUMO" sheetId="2" r:id="rId2"/>
+    <sheet name="ONSUMO2025" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="35">
   <si>
     <t>Fecha</t>
   </si>
@@ -128,6 +129,21 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Aceites Lubricantes</t>
+  </si>
+  <si>
+    <t>Bunker C o Fuel Oil</t>
+  </si>
+  <si>
+    <t>Gas Licuado de Petróleo</t>
+  </si>
+  <si>
+    <t>Grasas Lubricantes</t>
+  </si>
+  <si>
+    <t>Fecha, "Gasolina regular","Gasolina superior","Diesel alto azufre",]</t>
   </si>
 </sst>
 </file>
@@ -246,7 +262,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -283,6 +299,18 @@
     </xf>
     <xf numFmtId="4" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -621,13 +649,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78425B09-8B74-2C49-93AE-D8303799F11D}">
   <dimension ref="A1:Y289"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="76">
+    <row r="1" spans="1:25" ht="57">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -22925,12 +22953,12 @@
   <dimension ref="A1:X301"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:24" ht="32">
+    <row r="1" spans="1:24" ht="30">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -44704,6 +44732,353 @@
       <c r="X301" s="12">
         <f t="shared" si="2"/>
         <v>4477207.3100000005</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56EBC867-7A43-044F-8AA4-A081B1DCE829}">
+  <dimension ref="A1:R11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="7" max="7" width="22.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="76">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="14">
+        <v>45658</v>
+      </c>
+      <c r="B2" s="15">
+        <v>30930.87</v>
+      </c>
+      <c r="C2" s="15">
+        <v>356.8</v>
+      </c>
+      <c r="D2" s="15">
+        <v>100664.84</v>
+      </c>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15">
+        <v>84225.8</v>
+      </c>
+      <c r="G2" s="15">
+        <v>1326108.68</v>
+      </c>
+      <c r="H2" s="15">
+        <v>10019.4</v>
+      </c>
+      <c r="I2" s="15">
+        <v>512898.41</v>
+      </c>
+      <c r="J2" s="15">
+        <v>0</v>
+      </c>
+      <c r="K2" s="16">
+        <v>788005.35</v>
+      </c>
+      <c r="L2" s="16">
+        <v>645188.6</v>
+      </c>
+      <c r="M2" s="15">
+        <v>2409.5</v>
+      </c>
+      <c r="N2" s="16">
+        <v>5048.97</v>
+      </c>
+      <c r="O2" s="16">
+        <v>160.57</v>
+      </c>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15">
+        <v>3615</v>
+      </c>
+      <c r="R2" s="15">
+        <v>31785.360000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" s="14">
+        <v>45689</v>
+      </c>
+      <c r="B3" s="15">
+        <v>34736.14</v>
+      </c>
+      <c r="C3" s="15">
+        <v>5451.88</v>
+      </c>
+      <c r="D3" s="15">
+        <v>232009.89</v>
+      </c>
+      <c r="E3" s="15">
+        <v>2.75</v>
+      </c>
+      <c r="F3" s="15">
+        <v>88687.71</v>
+      </c>
+      <c r="G3" s="15">
+        <v>1102736.51</v>
+      </c>
+      <c r="H3" s="15">
+        <v>104468.41</v>
+      </c>
+      <c r="I3" s="15">
+        <v>858335.87</v>
+      </c>
+      <c r="J3" s="15">
+        <v>743.92</v>
+      </c>
+      <c r="K3" s="16">
+        <v>857375.76</v>
+      </c>
+      <c r="L3" s="16">
+        <v>686641.5</v>
+      </c>
+      <c r="M3" s="15">
+        <v>317.76</v>
+      </c>
+      <c r="N3" s="16">
+        <v>5899.4</v>
+      </c>
+      <c r="O3" s="16">
+        <v>40.01</v>
+      </c>
+      <c r="P3" s="15">
+        <v>515899.01</v>
+      </c>
+      <c r="Q3" s="15">
+        <v>3866</v>
+      </c>
+      <c r="R3" s="15">
+        <v>1449.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" s="14">
+        <v>45717</v>
+      </c>
+      <c r="B4" s="15">
+        <v>28820.59</v>
+      </c>
+      <c r="C4" s="15">
+        <v>9835.7000000000007</v>
+      </c>
+      <c r="D4" s="15">
+        <v>146856.64000000001</v>
+      </c>
+      <c r="E4" s="15">
+        <v>27.02</v>
+      </c>
+      <c r="F4" s="15">
+        <v>92922.69</v>
+      </c>
+      <c r="G4" s="15">
+        <v>1617427.16</v>
+      </c>
+      <c r="H4" s="15">
+        <v>6439.31</v>
+      </c>
+      <c r="I4" s="15">
+        <v>727180.68</v>
+      </c>
+      <c r="J4" s="15">
+        <v>11107.21</v>
+      </c>
+      <c r="K4" s="16">
+        <v>800182.17</v>
+      </c>
+      <c r="L4" s="16">
+        <v>796513.62</v>
+      </c>
+      <c r="M4" s="15">
+        <v>10867</v>
+      </c>
+      <c r="N4" s="16">
+        <v>4292.74</v>
+      </c>
+      <c r="O4" s="16">
+        <v>0.01</v>
+      </c>
+      <c r="P4" s="15">
+        <v>259102.01</v>
+      </c>
+      <c r="Q4" s="15">
+        <v>3930</v>
+      </c>
+      <c r="R4" s="15">
+        <v>14008.39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="14">
+        <v>45748</v>
+      </c>
+      <c r="B5" s="15">
+        <v>30215.71</v>
+      </c>
+      <c r="C5" s="15">
+        <v>6460.81</v>
+      </c>
+      <c r="D5" s="15">
+        <v>82574.399999999994</v>
+      </c>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15">
+        <v>66742.45</v>
+      </c>
+      <c r="G5" s="15">
+        <v>1226170.6200000001</v>
+      </c>
+      <c r="H5" s="15">
+        <v>75005.77</v>
+      </c>
+      <c r="I5" s="15">
+        <v>732805.98</v>
+      </c>
+      <c r="J5" s="15">
+        <v>699.08</v>
+      </c>
+      <c r="K5" s="16">
+        <v>898147.98</v>
+      </c>
+      <c r="L5" s="16">
+        <v>643476.9</v>
+      </c>
+      <c r="M5" s="15">
+        <v>696.44</v>
+      </c>
+      <c r="N5" s="16">
+        <v>5236.6499999999996</v>
+      </c>
+      <c r="O5" s="16">
+        <v>121.23</v>
+      </c>
+      <c r="P5" s="15">
+        <v>252344.01</v>
+      </c>
+      <c r="Q5" s="15">
+        <v>1113</v>
+      </c>
+      <c r="R5" s="15">
+        <v>26361.02</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="14">
+        <v>45778</v>
+      </c>
+      <c r="B6" s="15">
+        <v>35807.68</v>
+      </c>
+      <c r="C6" s="15">
+        <v>13165.63</v>
+      </c>
+      <c r="D6" s="15">
+        <v>182481.52</v>
+      </c>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15">
+        <v>70936.479999999996</v>
+      </c>
+      <c r="G6" s="15">
+        <v>1520640.21</v>
+      </c>
+      <c r="H6" s="15">
+        <v>5002.76</v>
+      </c>
+      <c r="I6" s="15">
+        <v>604722.9</v>
+      </c>
+      <c r="J6" s="15"/>
+      <c r="K6" s="16">
+        <v>785675.37</v>
+      </c>
+      <c r="L6" s="16">
+        <v>747443.53</v>
+      </c>
+      <c r="M6" s="15">
+        <v>593.63</v>
+      </c>
+      <c r="N6" s="16">
+        <v>5024.3999999999996</v>
+      </c>
+      <c r="O6" s="16">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15">
+        <v>2800</v>
+      </c>
+      <c r="R6" s="15">
+        <v>1731.21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="D11" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>